<commit_message>
changed from Lynda to LInkedIn, updated F2 problems, add IOT links to homepage
</commit_message>
<xml_diff>
--- a/Formative02/Formative02.xlsx
+++ b/Formative02/Formative02.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wp8798rh\Documents\MyWebSites\eProfessor\MIS362\Formative\Formative02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wp8798rh\OneDrive - MNSCU\GitHub\eprof1\MIS362-01\Formative02\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_C5089F65629FCEBEE634834F5FA033B13652DF75" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B94BCF55-A942-4032-9519-FDFC6301D76E}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="11760" windowHeight="7935" tabRatio="646"/>
+    <workbookView xWindow="360" yWindow="1224" windowWidth="11760" windowHeight="7932" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-NamedRanges" sheetId="1" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Total costs</t>
   </si>
@@ -98,9 +99,6 @@
     <t>Loan Term, Years</t>
   </si>
   <si>
-    <t>Montly Payment</t>
-  </si>
-  <si>
     <t>Real Gross National Product</t>
   </si>
   <si>
@@ -179,9 +177,6 @@
     <t>&lt;-- enter the formula for Profit using named ranges</t>
   </si>
   <si>
-    <t>&lt;-- enter the formula for cost using Vlookup</t>
-  </si>
-  <si>
     <t>&lt;-- enter the formula to calculate the monthly payment assuming future value is zero, and payments are made at the end of the period</t>
   </si>
   <si>
@@ -198,18 +193,45 @@
   </si>
   <si>
     <t>&lt;--</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Monthly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Tahoma"/>
+      </rPr>
+      <t xml:space="preserve"> Payment</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Cost of Ads</t>
+  </si>
+  <si>
+    <t>&lt;-- enter the formula for cost using Vlookup() and whatever else is needed</t>
+  </si>
+  <si>
+    <t>&lt;-- Average GNP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="Tahoma"/>
@@ -241,8 +263,19 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +300,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -285,7 +324,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -299,14 +338,18 @@
     <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Date" xfId="1"/>
-    <cellStyle name="Fixed" xfId="2"/>
+    <cellStyle name="Date" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Fixed" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Assignment02" xfId="3"/>
-    <cellStyle name="Normal_plr43Assignment01" xfId="4"/>
-    <cellStyle name="Text" xfId="5"/>
+    <cellStyle name="Normal_Assignment02" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal_plr43Assignment01" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Text" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -402,6 +445,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -437,6 +497,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,19 +689,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -632,7 +709,7 @@
         <v>540000</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -640,13 +717,13 @@
         <v>498000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -657,20 +734,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -678,7 +755,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -686,7 +763,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -694,44 +771,45 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
+    <row r="5" spans="1:3">
+      <c r="A5" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.08984375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="2.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="7.109375" style="1"/>
+    <col min="8" max="8" width="18.1796875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="7.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="21" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -745,7 +823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -759,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -773,7 +851,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -787,7 +865,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -801,7 +879,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="D6" s="1">
         <v>21</v>
       </c>
@@ -809,42 +887,42 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="D10" s="2">
         <v>3</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="D11" s="2">
         <v>7</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="D12" s="2">
         <v>13</v>
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="D13" s="2">
         <v>22</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="D14" s="2">
         <v>8</v>
       </c>
@@ -859,73 +937,73 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.08984375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="20.21875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" style="4" customWidth="1"/>
     <col min="2" max="2" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="7.109375" style="4"/>
+    <col min="3" max="3" width="5.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="7.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -935,9 +1013,9 @@
       <c r="I7" s="7"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -947,9 +1025,9 @@
       <c r="I8" s="7"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -959,9 +1037,9 @@
       <c r="I9" s="7"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -971,9 +1049,9 @@
       <c r="I10" s="7"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -983,9 +1061,9 @@
       <c r="I11" s="7"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -995,9 +1073,9 @@
       <c r="I12" s="7"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1007,9 +1085,9 @@
       <c r="I13" s="7"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1019,9 +1097,9 @@
       <c r="I14" s="7"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1031,9 +1109,9 @@
       <c r="I15" s="7"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1043,9 +1121,9 @@
       <c r="I16" s="7"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1055,9 +1133,9 @@
       <c r="I17" s="7"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1067,9 +1145,9 @@
       <c r="I18" s="7"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1079,9 +1157,9 @@
       <c r="I19" s="7"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1091,9 +1169,9 @@
       <c r="I20" s="7"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1103,9 +1181,9 @@
       <c r="I21" s="7"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1115,13 +1193,19 @@
       <c r="I22" s="7"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1132,24 +1216,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>689</v>
       </c>
@@ -1157,16 +1241,16 @@
         <v>1.99</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>170</v>
       </c>
@@ -1174,7 +1258,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1189</v>
       </c>
@@ -1182,7 +1266,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>892</v>
       </c>
@@ -1190,7 +1274,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>105</v>
       </c>
@@ -1198,7 +1282,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>763</v>
       </c>
@@ -1206,7 +1290,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>215</v>
       </c>
@@ -1214,7 +1298,7 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>239</v>
       </c>
@@ -1222,7 +1306,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>742</v>
       </c>
@@ -1230,7 +1314,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>890</v>
       </c>
@@ -1238,7 +1322,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>288</v>
       </c>
@@ -1246,7 +1330,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>802</v>
       </c>
@@ -1254,7 +1338,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>108</v>
       </c>
@@ -1262,7 +1346,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>118</v>
       </c>
@@ -1270,7 +1354,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>246</v>
       </c>
@@ -1278,7 +1362,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>1133</v>
       </c>
@@ -1286,7 +1370,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>160</v>
       </c>
@@ -1294,7 +1378,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>156</v>
       </c>
@@ -1302,7 +1386,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>143</v>
       </c>
@@ -1310,7 +1394,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>101</v>
       </c>
@@ -1318,7 +1402,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>201</v>
       </c>
@@ -1326,7 +1410,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>1083</v>
       </c>
@@ -1334,7 +1418,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>823</v>
       </c>
@@ -1342,7 +1426,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>462</v>
       </c>
@@ -1350,7 +1434,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>1046</v>
       </c>
@@ -1358,7 +1442,7 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>648</v>
       </c>
@@ -1366,7 +1450,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>705</v>
       </c>
@@ -1374,7 +1458,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>550</v>
       </c>
@@ -1382,7 +1466,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>314</v>
       </c>
@@ -1390,7 +1474,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>660</v>
       </c>
@@ -1398,7 +1482,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>571</v>
       </c>
@@ -1406,7 +1490,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>678</v>
       </c>
@@ -1414,7 +1498,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>1012</v>
       </c>
@@ -1422,7 +1506,7 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>1040</v>
       </c>
@@ -1430,7 +1514,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>752</v>
       </c>
@@ -1438,7 +1522,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>845</v>
       </c>
@@ -1446,7 +1530,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>829</v>
       </c>
@@ -1454,7 +1538,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>752</v>
       </c>
@@ -1462,7 +1546,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>1176</v>
       </c>
@@ -1470,7 +1554,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>749</v>
       </c>
@@ -1478,7 +1562,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>186</v>
       </c>
@@ -1486,7 +1570,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>237</v>
       </c>
@@ -1494,7 +1578,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>347</v>
       </c>
@@ -1502,7 +1586,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>692</v>
       </c>
@@ -1510,7 +1594,7 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>747</v>
       </c>
@@ -1518,7 +1602,7 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>794</v>
       </c>
@@ -1526,7 +1610,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>986</v>
       </c>
@@ -1534,7 +1618,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>1105</v>
       </c>
@@ -1542,7 +1626,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>1159</v>
       </c>
@@ -1550,7 +1634,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>873</v>
       </c>

</xml_diff>